<commit_message>
Uploaded with some analysis and updated the excel
</commit_message>
<xml_diff>
--- a/Boys Planet (EP1-5).xlsx
+++ b/Boys Planet (EP1-5).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Althea\Desktop\Coding\Boys planet visualization\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Althea\Desktop\Coding\Boys planet visualization\Boys-Planet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C29EAA-758F-4750-98B5-F87BFFD0A57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{034422D5-628F-4C86-B0B7-C2F43843A003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1044" yWindow="1044" windowWidth="12960" windowHeight="8160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="427">
   <si>
     <t>Name</t>
   </si>
@@ -1385,6 +1385,33 @@
   </si>
   <si>
     <t>Love Me Right - EXO (G)</t>
+  </si>
+  <si>
+    <t>Country (Map)</t>
+  </si>
+  <si>
+    <t>Japan</t>
+  </si>
+  <si>
+    <t>South Korea</t>
+  </si>
+  <si>
+    <t>Canada</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Taiwan</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Thailand</t>
   </si>
 </sst>
 </file>
@@ -7389,10 +7416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S94"/>
+  <dimension ref="A1:T94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="S1" sqref="S1:S1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7412,10 +7439,10 @@
     <col min="16" max="16" width="26.7109375" customWidth="1"/>
     <col min="17" max="17" width="17.5703125" customWidth="1"/>
     <col min="18" max="18" width="9.140625" customWidth="1"/>
-    <col min="19" max="19" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="17.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7473,8 +7500,11 @@
       <c r="S1" t="s">
         <v>400</v>
       </c>
+      <c r="T1" t="s">
+        <v>418</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -7529,11 +7559,14 @@
       <c r="R2" t="s">
         <v>402</v>
       </c>
-      <c r="S2" t="e" vm="1">
+      <c r="S2" t="s">
+        <v>419</v>
+      </c>
+      <c r="T2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>144</v>
       </c>
@@ -7588,11 +7621,14 @@
       <c r="R3" t="s">
         <v>401</v>
       </c>
-      <c r="S3" t="e" vm="2">
+      <c r="S3" t="s">
+        <v>420</v>
+      </c>
+      <c r="T3" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>234</v>
       </c>
@@ -7647,11 +7683,14 @@
       <c r="R4" t="s">
         <v>402</v>
       </c>
-      <c r="S4" t="e" vm="3">
+      <c r="S4" t="s">
+        <v>421</v>
+      </c>
+      <c r="T4" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>285</v>
       </c>
@@ -7706,11 +7745,14 @@
       <c r="R5" t="s">
         <v>402</v>
       </c>
-      <c r="S5" t="e" vm="4">
+      <c r="S5" t="s">
+        <v>422</v>
+      </c>
+      <c r="T5" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>138</v>
       </c>
@@ -7765,11 +7807,14 @@
       <c r="R6" t="s">
         <v>401</v>
       </c>
-      <c r="S6" t="e" vm="2">
+      <c r="S6" t="s">
+        <v>420</v>
+      </c>
+      <c r="T6" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>256</v>
       </c>
@@ -7824,11 +7869,14 @@
       <c r="R7" t="s">
         <v>402</v>
       </c>
-      <c r="S7" t="e" vm="4">
+      <c r="S7" t="s">
+        <v>422</v>
+      </c>
+      <c r="T7" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>150</v>
       </c>
@@ -7880,11 +7928,14 @@
       <c r="R8" t="s">
         <v>402</v>
       </c>
-      <c r="S8" t="e" vm="5">
+      <c r="S8" t="s">
+        <v>423</v>
+      </c>
+      <c r="T8" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>342</v>
       </c>
@@ -7921,11 +7972,14 @@
       <c r="R9" t="s">
         <v>402</v>
       </c>
-      <c r="S9" t="e" vm="4">
+      <c r="S9" t="s">
+        <v>422</v>
+      </c>
+      <c r="T9" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>341</v>
       </c>
@@ -7962,11 +8016,14 @@
       <c r="R10" t="s">
         <v>402</v>
       </c>
-      <c r="S10" t="e" vm="5">
+      <c r="S10" t="s">
+        <v>423</v>
+      </c>
+      <c r="T10" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>320</v>
       </c>
@@ -8006,11 +8063,14 @@
       <c r="R11" t="s">
         <v>402</v>
       </c>
-      <c r="S11" t="e" vm="4">
+      <c r="S11" t="s">
+        <v>422</v>
+      </c>
+      <c r="T11" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>348</v>
       </c>
@@ -8050,11 +8110,14 @@
       <c r="R12" t="s">
         <v>401</v>
       </c>
-      <c r="S12" t="e" vm="2">
+      <c r="S12" t="s">
+        <v>420</v>
+      </c>
+      <c r="T12" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>350</v>
       </c>
@@ -8094,11 +8157,14 @@
       <c r="R13" t="s">
         <v>401</v>
       </c>
-      <c r="S13" t="e" vm="2">
+      <c r="S13" t="s">
+        <v>420</v>
+      </c>
+      <c r="T13" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>290</v>
       </c>
@@ -8153,11 +8219,14 @@
       <c r="R14" t="s">
         <v>401</v>
       </c>
-      <c r="S14" t="e" vm="2">
+      <c r="S14" t="s">
+        <v>420</v>
+      </c>
+      <c r="T14" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>201</v>
       </c>
@@ -8209,11 +8278,14 @@
       <c r="R15" t="s">
         <v>402</v>
       </c>
-      <c r="S15" t="e" vm="6">
+      <c r="S15" t="s">
+        <v>424</v>
+      </c>
+      <c r="T15" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>190</v>
       </c>
@@ -8268,11 +8340,14 @@
       <c r="R16" t="s">
         <v>402</v>
       </c>
-      <c r="S16" t="e" vm="6">
+      <c r="S16" t="s">
+        <v>424</v>
+      </c>
+      <c r="T16" t="e" vm="6">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>317</v>
       </c>
@@ -8312,11 +8387,14 @@
       <c r="R17" t="s">
         <v>402</v>
       </c>
-      <c r="S17" t="e" vm="5">
+      <c r="S17" t="s">
+        <v>423</v>
+      </c>
+      <c r="T17" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>331</v>
       </c>
@@ -8356,11 +8434,14 @@
       <c r="R18" t="s">
         <v>402</v>
       </c>
-      <c r="S18" t="e" vm="4">
+      <c r="S18" t="s">
+        <v>422</v>
+      </c>
+      <c r="T18" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>332</v>
       </c>
@@ -8400,11 +8481,14 @@
       <c r="R19" t="s">
         <v>401</v>
       </c>
-      <c r="S19" t="e" vm="2">
+      <c r="S19" t="s">
+        <v>420</v>
+      </c>
+      <c r="T19" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -8459,11 +8543,14 @@
       <c r="R20" t="s">
         <v>401</v>
       </c>
-      <c r="S20" t="e" vm="2">
+      <c r="S20" t="s">
+        <v>420</v>
+      </c>
+      <c r="T20" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>323</v>
       </c>
@@ -8503,11 +8590,14 @@
       <c r="R21" t="s">
         <v>401</v>
       </c>
-      <c r="S21" t="e" vm="2">
+      <c r="S21" t="s">
+        <v>420</v>
+      </c>
+      <c r="T21" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>338</v>
       </c>
@@ -8544,11 +8634,14 @@
       <c r="R22" t="s">
         <v>402</v>
       </c>
-      <c r="S22" t="e" vm="1">
+      <c r="S22" t="s">
+        <v>419</v>
+      </c>
+      <c r="T22" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>93</v>
       </c>
@@ -8603,11 +8696,14 @@
       <c r="R23" t="s">
         <v>402</v>
       </c>
-      <c r="S23" t="e" vm="1">
+      <c r="S23" t="s">
+        <v>419</v>
+      </c>
+      <c r="T23" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>121</v>
       </c>
@@ -8662,11 +8758,14 @@
       <c r="R24" t="s">
         <v>402</v>
       </c>
-      <c r="S24" t="e" vm="1">
+      <c r="S24" t="s">
+        <v>419</v>
+      </c>
+      <c r="T24" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>322</v>
       </c>
@@ -8706,11 +8805,14 @@
       <c r="R25" t="s">
         <v>401</v>
       </c>
-      <c r="S25" t="e" vm="2">
+      <c r="S25" t="s">
+        <v>420</v>
+      </c>
+      <c r="T25" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>324</v>
       </c>
@@ -8750,11 +8852,14 @@
       <c r="R26" t="s">
         <v>402</v>
       </c>
-      <c r="S26" t="e" vm="1">
+      <c r="S26" t="s">
+        <v>419</v>
+      </c>
+      <c r="T26" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>357</v>
       </c>
@@ -8794,11 +8899,14 @@
       <c r="R27" t="s">
         <v>402</v>
       </c>
-      <c r="S27" t="e" vm="1">
+      <c r="S27" t="s">
+        <v>419</v>
+      </c>
+      <c r="T27" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>326</v>
       </c>
@@ -8838,11 +8946,14 @@
       <c r="R28" t="s">
         <v>402</v>
       </c>
-      <c r="S28" t="e" vm="1">
+      <c r="S28" t="s">
+        <v>419</v>
+      </c>
+      <c r="T28" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>335</v>
       </c>
@@ -8882,11 +8993,14 @@
       <c r="R29" t="s">
         <v>401</v>
       </c>
-      <c r="S29" t="e" vm="2">
+      <c r="S29" t="s">
+        <v>420</v>
+      </c>
+      <c r="T29" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>334</v>
       </c>
@@ -8926,11 +9040,14 @@
       <c r="R30" t="s">
         <v>401</v>
       </c>
-      <c r="S30" t="e" vm="2">
+      <c r="S30" t="s">
+        <v>420</v>
+      </c>
+      <c r="T30" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -8985,11 +9102,14 @@
       <c r="R31" t="s">
         <v>402</v>
       </c>
-      <c r="S31" t="e" vm="7">
+      <c r="S31" t="s">
+        <v>425</v>
+      </c>
+      <c r="T31" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>343</v>
       </c>
@@ -9029,11 +9149,14 @@
       <c r="R32" t="s">
         <v>401</v>
       </c>
-      <c r="S32" t="e" vm="2">
+      <c r="S32" t="s">
+        <v>420</v>
+      </c>
+      <c r="T32" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>339</v>
       </c>
@@ -9073,11 +9196,14 @@
       <c r="R33" t="s">
         <v>401</v>
       </c>
-      <c r="S33" t="e" vm="2">
+      <c r="S33" t="s">
+        <v>420</v>
+      </c>
+      <c r="T33" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>296</v>
       </c>
@@ -9129,11 +9255,14 @@
       <c r="R34" t="s">
         <v>401</v>
       </c>
-      <c r="S34" t="e" vm="2">
+      <c r="S34" t="s">
+        <v>420</v>
+      </c>
+      <c r="T34" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>267</v>
       </c>
@@ -9188,11 +9317,14 @@
       <c r="R35" t="s">
         <v>401</v>
       </c>
-      <c r="S35" t="e" vm="2">
+      <c r="S35" t="s">
+        <v>420</v>
+      </c>
+      <c r="T35" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>337</v>
       </c>
@@ -9229,11 +9361,14 @@
       <c r="R36" t="s">
         <v>401</v>
       </c>
-      <c r="S36" t="e" vm="2">
+      <c r="S36" t="s">
+        <v>420</v>
+      </c>
+      <c r="T36" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>156</v>
       </c>
@@ -9288,11 +9423,14 @@
       <c r="R37" t="s">
         <v>401</v>
       </c>
-      <c r="S37" t="e" vm="2">
+      <c r="S37" t="s">
+        <v>420</v>
+      </c>
+      <c r="T37" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>346</v>
       </c>
@@ -9332,11 +9470,14 @@
       <c r="R38" t="s">
         <v>401</v>
       </c>
-      <c r="S38" t="e" vm="2">
+      <c r="S38" t="s">
+        <v>420</v>
+      </c>
+      <c r="T38" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>325</v>
       </c>
@@ -9376,11 +9517,14 @@
       <c r="R39" t="s">
         <v>402</v>
       </c>
-      <c r="S39" t="e" vm="1">
+      <c r="S39" t="s">
+        <v>419</v>
+      </c>
+      <c r="T39" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>48</v>
       </c>
@@ -9435,11 +9579,14 @@
       <c r="R40" t="s">
         <v>402</v>
       </c>
-      <c r="S40" t="e" vm="1">
+      <c r="S40" t="s">
+        <v>419</v>
+      </c>
+      <c r="T40" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>36</v>
       </c>
@@ -9494,11 +9641,14 @@
       <c r="R41" t="s">
         <v>401</v>
       </c>
-      <c r="S41" t="e" vm="2">
+      <c r="S41" t="s">
+        <v>420</v>
+      </c>
+      <c r="T41" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>18</v>
       </c>
@@ -9553,11 +9703,14 @@
       <c r="R42" t="s">
         <v>401</v>
       </c>
-      <c r="S42" t="e" vm="2">
+      <c r="S42" t="s">
+        <v>420</v>
+      </c>
+      <c r="T42" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>347</v>
       </c>
@@ -9594,11 +9747,14 @@
       <c r="R43" t="s">
         <v>401</v>
       </c>
-      <c r="S43" t="e" vm="2">
+      <c r="S43" t="s">
+        <v>420</v>
+      </c>
+      <c r="T43" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>351</v>
       </c>
@@ -9638,11 +9794,14 @@
       <c r="R44" t="s">
         <v>401</v>
       </c>
-      <c r="S44" t="e" vm="2">
+      <c r="S44" t="s">
+        <v>420</v>
+      </c>
+      <c r="T44" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>65</v>
       </c>
@@ -9697,11 +9856,14 @@
       <c r="R45" t="s">
         <v>401</v>
       </c>
-      <c r="S45" t="e" vm="2">
+      <c r="S45" t="s">
+        <v>420</v>
+      </c>
+      <c r="T45" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>211</v>
       </c>
@@ -9753,11 +9915,14 @@
       <c r="R46" t="s">
         <v>402</v>
       </c>
-      <c r="S46" t="e" vm="4">
+      <c r="S46" t="s">
+        <v>422</v>
+      </c>
+      <c r="T46" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>82</v>
       </c>
@@ -9812,11 +9977,14 @@
       <c r="R47" t="s">
         <v>401</v>
       </c>
-      <c r="S47" t="e" vm="2">
+      <c r="S47" t="s">
+        <v>420</v>
+      </c>
+      <c r="T47" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>76</v>
       </c>
@@ -9871,11 +10039,14 @@
       <c r="R48" t="s">
         <v>401</v>
       </c>
-      <c r="S48" t="e" vm="2">
+      <c r="S48" t="s">
+        <v>420</v>
+      </c>
+      <c r="T48" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>273</v>
       </c>
@@ -9930,11 +10101,14 @@
       <c r="R49" t="s">
         <v>401</v>
       </c>
-      <c r="S49" t="e" vm="2">
+      <c r="S49" t="s">
+        <v>420</v>
+      </c>
+      <c r="T49" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>228</v>
       </c>
@@ -9989,11 +10163,14 @@
       <c r="R50" t="s">
         <v>401</v>
       </c>
-      <c r="S50" t="e" vm="2">
+      <c r="S50" t="s">
+        <v>420</v>
+      </c>
+      <c r="T50" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>42</v>
       </c>
@@ -10048,11 +10225,14 @@
       <c r="R51" t="s">
         <v>401</v>
       </c>
-      <c r="S51" t="e" vm="2">
+      <c r="S51" t="s">
+        <v>420</v>
+      </c>
+      <c r="T51" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>261</v>
       </c>
@@ -10107,11 +10287,14 @@
       <c r="R52" t="s">
         <v>401</v>
       </c>
-      <c r="S52" t="e" vm="2">
+      <c r="S52" t="s">
+        <v>420</v>
+      </c>
+      <c r="T52" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>222</v>
       </c>
@@ -10166,11 +10349,14 @@
       <c r="R53" t="s">
         <v>401</v>
       </c>
-      <c r="S53" t="e" vm="2">
+      <c r="S53" t="s">
+        <v>420</v>
+      </c>
+      <c r="T53" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>115</v>
       </c>
@@ -10222,11 +10408,14 @@
       <c r="R54" t="s">
         <v>401</v>
       </c>
-      <c r="S54" t="e" vm="2">
+      <c r="S54" t="s">
+        <v>420</v>
+      </c>
+      <c r="T54" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>239</v>
       </c>
@@ -10281,11 +10470,14 @@
       <c r="R55" t="s">
         <v>401</v>
       </c>
-      <c r="S55" t="e" vm="2">
+      <c r="S55" t="s">
+        <v>420</v>
+      </c>
+      <c r="T55" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>173</v>
       </c>
@@ -10340,11 +10532,14 @@
       <c r="R56" t="s">
         <v>401</v>
       </c>
-      <c r="S56" t="e" vm="2">
+      <c r="S56" t="s">
+        <v>420</v>
+      </c>
+      <c r="T56" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>330</v>
       </c>
@@ -10381,11 +10576,14 @@
       <c r="R57" t="s">
         <v>402</v>
       </c>
-      <c r="S57" t="e" vm="4">
+      <c r="S57" t="s">
+        <v>422</v>
+      </c>
+      <c r="T57" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>184</v>
       </c>
@@ -10437,11 +10635,14 @@
       <c r="R58" t="s">
         <v>402</v>
       </c>
-      <c r="S58" t="e" vm="4">
+      <c r="S58" t="s">
+        <v>422</v>
+      </c>
+      <c r="T58" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>352</v>
       </c>
@@ -10481,11 +10682,14 @@
       <c r="R59" t="s">
         <v>402</v>
       </c>
-      <c r="S59" t="e" vm="8">
+      <c r="S59" t="s">
+        <v>426</v>
+      </c>
+      <c r="T59" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>132</v>
       </c>
@@ -10540,11 +10744,14 @@
       <c r="R60" t="s">
         <v>401</v>
       </c>
-      <c r="S60" t="e" vm="2">
+      <c r="S60" t="s">
+        <v>420</v>
+      </c>
+      <c r="T60" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>179</v>
       </c>
@@ -10599,11 +10806,14 @@
       <c r="R61" t="s">
         <v>402</v>
       </c>
-      <c r="S61" t="e" vm="7">
+      <c r="S61" t="s">
+        <v>425</v>
+      </c>
+      <c r="T61" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>316</v>
       </c>
@@ -10640,11 +10850,14 @@
       <c r="R62" t="s">
         <v>402</v>
       </c>
-      <c r="S62" t="e" vm="8">
+      <c r="S62" t="s">
+        <v>426</v>
+      </c>
+      <c r="T62" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>195</v>
       </c>
@@ -10699,11 +10912,14 @@
       <c r="R63" t="s">
         <v>401</v>
       </c>
-      <c r="S63" t="e" vm="2">
+      <c r="S63" t="s">
+        <v>420</v>
+      </c>
+      <c r="T63" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>162</v>
       </c>
@@ -10758,11 +10974,14 @@
       <c r="R64" t="s">
         <v>402</v>
       </c>
-      <c r="S64" t="e" vm="4">
+      <c r="S64" t="s">
+        <v>422</v>
+      </c>
+      <c r="T64" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>321</v>
       </c>
@@ -10799,11 +11018,14 @@
       <c r="R65" t="s">
         <v>402</v>
       </c>
-      <c r="S65" t="e" vm="1">
+      <c r="S65" t="s">
+        <v>419</v>
+      </c>
+      <c r="T65" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>344</v>
       </c>
@@ -10843,11 +11065,14 @@
       <c r="R66" t="s">
         <v>402</v>
       </c>
-      <c r="S66" t="e" vm="1">
+      <c r="S66" t="s">
+        <v>419</v>
+      </c>
+      <c r="T66" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>59</v>
       </c>
@@ -10902,11 +11127,14 @@
       <c r="R67" t="s">
         <v>401</v>
       </c>
-      <c r="S67" t="e" vm="2">
+      <c r="S67" t="s">
+        <v>420</v>
+      </c>
+      <c r="T67" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>340</v>
       </c>
@@ -10943,11 +11171,14 @@
       <c r="R68" t="s">
         <v>401</v>
       </c>
-      <c r="S68" t="e" vm="2">
+      <c r="S68" t="s">
+        <v>420</v>
+      </c>
+      <c r="T68" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>126</v>
       </c>
@@ -11002,11 +11233,14 @@
       <c r="R69" t="s">
         <v>401</v>
       </c>
-      <c r="S69" t="e" vm="2">
+      <c r="S69" t="s">
+        <v>420</v>
+      </c>
+      <c r="T69" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>279</v>
       </c>
@@ -11061,11 +11295,14 @@
       <c r="R70" t="s">
         <v>401</v>
       </c>
-      <c r="S70" t="e" vm="2">
+      <c r="S70" t="s">
+        <v>420</v>
+      </c>
+      <c r="T70" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>250</v>
       </c>
@@ -11120,11 +11357,14 @@
       <c r="R71" t="s">
         <v>401</v>
       </c>
-      <c r="S71" t="e" vm="2">
+      <c r="S71" t="s">
+        <v>420</v>
+      </c>
+      <c r="T71" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="72" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>333</v>
       </c>
@@ -11164,11 +11404,14 @@
       <c r="R72" t="s">
         <v>401</v>
       </c>
-      <c r="S72" t="e" vm="2">
+      <c r="S72" t="s">
+        <v>420</v>
+      </c>
+      <c r="T72" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="73" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>319</v>
       </c>
@@ -11208,11 +11451,14 @@
       <c r="R73" t="s">
         <v>402</v>
       </c>
-      <c r="S73" t="e" vm="5">
+      <c r="S73" t="s">
+        <v>423</v>
+      </c>
+      <c r="T73" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="74" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>71</v>
       </c>
@@ -11267,11 +11513,14 @@
       <c r="R74" t="s">
         <v>402</v>
       </c>
-      <c r="S74" t="e" vm="4">
+      <c r="S74" t="s">
+        <v>422</v>
+      </c>
+      <c r="T74" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="75" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>329</v>
       </c>
@@ -11308,11 +11557,14 @@
       <c r="R75" t="s">
         <v>402</v>
       </c>
-      <c r="S75" t="e" vm="1">
+      <c r="S75" t="s">
+        <v>419</v>
+      </c>
+      <c r="T75" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="76" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>104</v>
       </c>
@@ -11367,11 +11619,14 @@
       <c r="R76" t="s">
         <v>401</v>
       </c>
-      <c r="S76" t="e" vm="2">
+      <c r="S76" t="s">
+        <v>420</v>
+      </c>
+      <c r="T76" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="77" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>12</v>
       </c>
@@ -11426,11 +11681,14 @@
       <c r="R77" t="s">
         <v>402</v>
       </c>
-      <c r="S77" t="e" vm="3">
+      <c r="S77" t="s">
+        <v>421</v>
+      </c>
+      <c r="T77" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="78" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>6</v>
       </c>
@@ -11485,11 +11743,14 @@
       <c r="R78" t="s">
         <v>401</v>
       </c>
-      <c r="S78" t="e" vm="2">
+      <c r="S78" t="s">
+        <v>420</v>
+      </c>
+      <c r="T78" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="79" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>88</v>
       </c>
@@ -11544,11 +11805,14 @@
       <c r="R79" t="s">
         <v>402</v>
       </c>
-      <c r="S79" t="e" vm="1">
+      <c r="S79" t="s">
+        <v>419</v>
+      </c>
+      <c r="T79" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="80" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>327</v>
       </c>
@@ -11588,11 +11852,14 @@
       <c r="R80" t="s">
         <v>402</v>
       </c>
-      <c r="S80" t="e" vm="1">
+      <c r="S80" t="s">
+        <v>419</v>
+      </c>
+      <c r="T80" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="81" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>315</v>
       </c>
@@ -11632,11 +11899,14 @@
       <c r="R81" t="s">
         <v>402</v>
       </c>
-      <c r="S81" t="e" vm="4">
+      <c r="S81" t="s">
+        <v>422</v>
+      </c>
+      <c r="T81" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>167</v>
       </c>
@@ -11691,11 +11961,14 @@
       <c r="R82" t="s">
         <v>402</v>
       </c>
-      <c r="S82" t="e" vm="4">
+      <c r="S82" t="s">
+        <v>422</v>
+      </c>
+      <c r="T82" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>349</v>
       </c>
@@ -11732,11 +12005,14 @@
       <c r="R83" t="s">
         <v>402</v>
       </c>
-      <c r="S83" t="e" vm="4">
+      <c r="S83" t="s">
+        <v>422</v>
+      </c>
+      <c r="T83" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="84" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>318</v>
       </c>
@@ -11776,11 +12052,14 @@
       <c r="R84" t="s">
         <v>402</v>
       </c>
-      <c r="S84" t="e" vm="8">
+      <c r="S84" t="s">
+        <v>426</v>
+      </c>
+      <c r="T84" t="e" vm="8">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>245</v>
       </c>
@@ -11835,11 +12114,14 @@
       <c r="R85" t="s">
         <v>402</v>
       </c>
-      <c r="S85" t="e" vm="4">
+      <c r="S85" t="s">
+        <v>422</v>
+      </c>
+      <c r="T85" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>307</v>
       </c>
@@ -11894,11 +12176,14 @@
       <c r="R86" t="s">
         <v>402</v>
       </c>
-      <c r="S86" t="e" vm="4">
+      <c r="S86" t="s">
+        <v>422</v>
+      </c>
+      <c r="T86" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>345</v>
       </c>
@@ -11938,11 +12223,14 @@
       <c r="R87" t="s">
         <v>402</v>
       </c>
-      <c r="S87" t="e" vm="4">
+      <c r="S87" t="s">
+        <v>422</v>
+      </c>
+      <c r="T87" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>98</v>
       </c>
@@ -11997,11 +12285,14 @@
       <c r="R88" t="s">
         <v>401</v>
       </c>
-      <c r="S88" t="e" vm="2">
+      <c r="S88" t="s">
+        <v>420</v>
+      </c>
+      <c r="T88" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>216</v>
       </c>
@@ -12053,11 +12344,14 @@
       <c r="R89" t="s">
         <v>401</v>
       </c>
-      <c r="S89" t="e" vm="2">
+      <c r="S89" t="s">
+        <v>420</v>
+      </c>
+      <c r="T89" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="90" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>302</v>
       </c>
@@ -12109,11 +12403,14 @@
       <c r="R90" t="s">
         <v>402</v>
       </c>
-      <c r="S90" t="e" vm="1">
+      <c r="S90" t="s">
+        <v>419</v>
+      </c>
+      <c r="T90" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="91" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>336</v>
       </c>
@@ -12150,11 +12447,14 @@
       <c r="R91" t="s">
         <v>402</v>
       </c>
-      <c r="S91" t="e" vm="1">
+      <c r="S91" t="s">
+        <v>419</v>
+      </c>
+      <c r="T91" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>328</v>
       </c>
@@ -12191,11 +12491,14 @@
       <c r="R92" t="s">
         <v>402</v>
       </c>
-      <c r="S92" t="e" vm="1">
+      <c r="S92" t="s">
+        <v>419</v>
+      </c>
+      <c r="T92" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>30</v>
       </c>
@@ -12250,11 +12553,14 @@
       <c r="R93" t="s">
         <v>402</v>
       </c>
-      <c r="S93" t="e" vm="4">
+      <c r="S93" t="s">
+        <v>422</v>
+      </c>
+      <c r="T93" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="94" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>206</v>
       </c>
@@ -12309,7 +12615,10 @@
       <c r="R94" t="s">
         <v>402</v>
       </c>
-      <c r="S94" t="e" vm="4">
+      <c r="S94" t="s">
+        <v>422</v>
+      </c>
+      <c r="T94" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
     </row>

</xml_diff>